<commit_message>
Final Code with JSON
</commit_message>
<xml_diff>
--- a/Duplicate Data.xlsx
+++ b/Duplicate Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="301">
   <si>
     <t>Company</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Twitter Account Age (Years)</t>
+  </si>
+  <si>
+    <t>Nifty 50 Stock</t>
   </si>
   <si>
     <t>Kratos Energy &amp; Infrastructure Ltd.</t>
@@ -1290,13 +1293,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS4"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:46">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1429,22 +1432,25 @@
       <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:45">
+      <c r="AT1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46">
       <c r="A2" s="1">
         <v>2045</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>501261</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" s="2">
         <v>44389</v>
@@ -1498,30 +1504,30 @@
         <v>0</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AM2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46">
       <c r="A3" s="1">
         <v>3239</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H3" s="2">
         <v>44673</v>
@@ -1578,48 +1584,48 @@
         <v>0</v>
       </c>
       <c r="AK3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AM3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AO3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AP3">
         <v>8</v>
       </c>
       <c r="AQ3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AR3" s="2">
         <v>42849</v>
       </c>
       <c r="AS3">
-        <v>5.080555555555556</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45">
+        <v>5.086111111111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46">
       <c r="A4" s="1">
         <v>3720</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>539574</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H4" s="2">
         <v>44620</v>
@@ -1679,13 +1685,13 @@
         <v>0</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AM4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1712,40 +1718,40 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1753,7 +1759,7 @@
         <v>802</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F2">
         <v>77.11442786000001</v>
@@ -1773,7 +1779,7 @@
         <v>946</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>18.32359584</v>
@@ -1811,7 +1817,7 @@
         <v>1065</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4">
         <v>18.56829477</v>
@@ -1846,7 +1852,7 @@
         <v>1238</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>39.58011923</v>
@@ -1884,7 +1890,7 @@
         <v>1278</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>73.65689144</v>
@@ -1913,7 +1919,7 @@
         <v>1281</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D7">
         <v>16.68377208</v>
@@ -1951,7 +1957,7 @@
         <v>1291</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1962,7 +1968,7 @@
         <v>1314</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F9">
         <v>72.52884615000001</v>
@@ -1991,7 +1997,7 @@
         <v>1396</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D10">
         <v>53.69102847</v>
@@ -2029,7 +2035,7 @@
         <v>1406</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11">
         <v>74.79879787</v>
@@ -2067,7 +2073,7 @@
         <v>1483</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -2081,7 +2087,7 @@
         <v>1527</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E13">
         <v>31.66172745</v>
@@ -2113,7 +2119,7 @@
         <v>1577</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -2127,7 +2133,7 @@
         <v>1594</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F15">
         <v>72.22111445</v>
@@ -2156,7 +2162,7 @@
         <v>1624</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D16">
         <v>14.26175152</v>
@@ -2194,7 +2200,7 @@
         <v>1626</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D17">
         <v>8.711379163</v>
@@ -2232,7 +2238,7 @@
         <v>1638</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18">
         <v>9.711993092</v>
@@ -2270,7 +2276,7 @@
         <v>1675</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19">
         <v>35.92617686</v>
@@ -2308,7 +2314,7 @@
         <v>1778</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20">
         <v>100</v>
@@ -2337,7 +2343,7 @@
         <v>1781</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21">
         <v>24.45682254</v>
@@ -2375,7 +2381,7 @@
         <v>1798</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F22">
         <v>90.08104879</v>
@@ -2404,7 +2410,7 @@
         <v>1799</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F23">
         <v>60.55930502</v>
@@ -2433,7 +2439,7 @@
         <v>1800</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D24">
         <v>25.27584744</v>
@@ -2471,7 +2477,7 @@
         <v>1805</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F25">
         <v>70.20059141</v>
@@ -2500,7 +2506,7 @@
         <v>1835</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F26">
         <v>73.46892398999999</v>
@@ -2529,7 +2535,7 @@
         <v>1839</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D27">
         <v>19.89553005</v>
@@ -2567,7 +2573,7 @@
         <v>1859</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2581,7 +2587,7 @@
         <v>1869</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D29">
         <v>13.44797022</v>
@@ -2619,7 +2625,7 @@
         <v>1901</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F30">
         <v>41.8822023</v>
@@ -2648,7 +2654,7 @@
         <v>1921</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D31">
         <v>9.629430517999999</v>
@@ -2686,7 +2692,7 @@
         <v>1962</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D32">
         <v>13.75875696</v>
@@ -2724,7 +2730,7 @@
         <v>1999</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D33">
         <v>2.142089721</v>
@@ -2762,7 +2768,7 @@
         <v>2020</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E34">
         <v>-15.04124228</v>
@@ -2791,7 +2797,7 @@
         <v>2041</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D35">
         <v>18.74385646</v>
@@ -2829,7 +2835,7 @@
         <v>2050</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F36">
         <v>73.37526205</v>
@@ -2858,7 +2864,7 @@
         <v>2077</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D37">
         <v>11.92397139</v>
@@ -2896,7 +2902,7 @@
         <v>2088</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -2910,7 +2916,7 @@
         <v>2104</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D39">
         <v>26.15779591</v>
@@ -2948,7 +2954,7 @@
         <v>2107</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F40">
         <v>73.62927083</v>
@@ -2977,7 +2983,7 @@
         <v>2116</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D41">
         <v>10.6434075</v>
@@ -3015,7 +3021,7 @@
         <v>2178</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F42">
         <v>71.33271199000001</v>
@@ -3047,7 +3053,7 @@
         <v>2214</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D43">
         <v>14.69974251</v>
@@ -3085,7 +3091,7 @@
         <v>2215</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D44">
         <v>15.27442835</v>
@@ -3123,7 +3129,7 @@
         <v>2229</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -3137,7 +3143,7 @@
         <v>2230</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F46">
         <v>69.98340439</v>
@@ -3169,7 +3175,7 @@
         <v>2236</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D47">
         <v>24.48812691</v>
@@ -3204,7 +3210,7 @@
         <v>2269</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D48">
         <v>17.40111849</v>
@@ -3242,7 +3248,7 @@
         <v>2293</v>
       </c>
       <c r="B49" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D49">
         <v>20.72281664</v>
@@ -3280,7 +3286,7 @@
         <v>2317</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D50">
         <v>13.55002685</v>
@@ -3318,7 +3324,7 @@
         <v>2331</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F51">
         <v>73.46146154</v>
@@ -3347,7 +3353,7 @@
         <v>2356</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F52">
         <v>73.52941176</v>
@@ -3376,7 +3382,7 @@
         <v>2378</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D53">
         <v>-16.29930059</v>
@@ -3414,7 +3420,7 @@
         <v>2416</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D54">
         <v>18.24922467</v>
@@ -3452,7 +3458,7 @@
         <v>2438</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D55">
         <v>17.12555025</v>
@@ -3490,7 +3496,7 @@
         <v>2453</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D56">
         <v>13.65582104</v>
@@ -3528,7 +3534,7 @@
         <v>2454</v>
       </c>
       <c r="B57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F57">
         <v>69.86564798000001</v>
@@ -3557,7 +3563,7 @@
         <v>2464</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F58">
         <v>50.6108843</v>
@@ -3589,7 +3595,7 @@
         <v>2466</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F59">
         <v>71.21870504</v>
@@ -3618,7 +3624,7 @@
         <v>2475</v>
       </c>
       <c r="B60" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D60">
         <v>37.53437714</v>
@@ -3656,7 +3662,7 @@
         <v>2477</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D61">
         <v>9.040537072999999</v>
@@ -3694,7 +3700,7 @@
         <v>2481</v>
       </c>
       <c r="B62" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D62">
         <v>15.06821554</v>
@@ -3732,7 +3738,7 @@
         <v>2483</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D63">
         <v>22.48507297</v>
@@ -3770,7 +3776,7 @@
         <v>2509</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D64">
         <v>10.27975702</v>
@@ -3808,7 +3814,7 @@
         <v>2519</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D65">
         <v>13.24829479</v>
@@ -3846,7 +3852,7 @@
         <v>2527</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D66">
         <v>2.789274173</v>
@@ -3884,10 +3890,10 @@
         <v>2532</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C67" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D67">
         <v>12.76128466</v>
@@ -3925,7 +3931,7 @@
         <v>2541</v>
       </c>
       <c r="B68" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D68">
         <v>23.19368602</v>
@@ -3963,7 +3969,7 @@
         <v>2552</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D69">
         <v>11.33974215</v>
@@ -4001,7 +4007,7 @@
         <v>2579</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D70">
         <v>6.085949823</v>
@@ -4039,7 +4045,7 @@
         <v>2585</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F71">
         <v>60</v>
@@ -4071,7 +4077,7 @@
         <v>2591</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D72">
         <v>16.73576793</v>
@@ -4109,7 +4115,7 @@
         <v>2594</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D73">
         <v>11.76755414</v>
@@ -4147,7 +4153,7 @@
         <v>2612</v>
       </c>
       <c r="B74" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I74">
         <v>0</v>
@@ -4158,7 +4164,7 @@
         <v>2616</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F75">
         <v>67.54874651999999</v>
@@ -4187,7 +4193,7 @@
         <v>2640</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -4198,7 +4204,7 @@
         <v>2658</v>
       </c>
       <c r="B77" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D77">
         <v>17.11081015</v>
@@ -4236,7 +4242,7 @@
         <v>2668</v>
       </c>
       <c r="B78" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F78">
         <v>34.91323527</v>
@@ -4265,7 +4271,7 @@
         <v>2669</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D79">
         <v>12.79086413</v>
@@ -4303,7 +4309,7 @@
         <v>2688</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D80">
         <v>24.37971925</v>
@@ -4341,7 +4347,7 @@
         <v>2695</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D81">
         <v>8.877874373999999</v>
@@ -4379,10 +4385,10 @@
         <v>2700</v>
       </c>
       <c r="B82" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C82" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D82">
         <v>1.079062619</v>
@@ -4420,7 +4426,7 @@
         <v>2702</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D83">
         <v>-1.59178347</v>
@@ -4458,7 +4464,7 @@
         <v>2714</v>
       </c>
       <c r="B84" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F84">
         <v>73.30603753</v>
@@ -4487,7 +4493,7 @@
         <v>2715</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D85">
         <v>12.08997479</v>
@@ -4525,7 +4531,7 @@
         <v>2735</v>
       </c>
       <c r="B86" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I86">
         <v>0</v>
@@ -4539,7 +4545,7 @@
         <v>2748</v>
       </c>
       <c r="B87" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F87">
         <v>73.39950372</v>
@@ -4568,7 +4574,7 @@
         <v>2752</v>
       </c>
       <c r="B88" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D88">
         <v>-7.987723809</v>
@@ -4606,7 +4612,7 @@
         <v>2767</v>
       </c>
       <c r="B89" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D89">
         <v>13.83142391</v>
@@ -4644,7 +4650,7 @@
         <v>2788</v>
       </c>
       <c r="B90" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F90">
         <v>73.30047949</v>
@@ -4673,7 +4679,7 @@
         <v>2812</v>
       </c>
       <c r="B91" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I91">
         <v>0</v>
@@ -4687,7 +4693,7 @@
         <v>2833</v>
       </c>
       <c r="B92" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D92">
         <v>-10.68124605</v>
@@ -4725,7 +4731,7 @@
         <v>2837</v>
       </c>
       <c r="B93" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D93">
         <v>6.956863173</v>
@@ -4763,7 +4769,7 @@
         <v>2839</v>
       </c>
       <c r="B94" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D94">
         <v>8.057748638</v>
@@ -4801,7 +4807,7 @@
         <v>2840</v>
       </c>
       <c r="B95" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F95">
         <v>72.10682493</v>
@@ -4830,7 +4836,7 @@
         <v>2857</v>
       </c>
       <c r="B96" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D96">
         <v>23.86164937</v>
@@ -4865,7 +4871,7 @@
         <v>2867</v>
       </c>
       <c r="B97" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D97">
         <v>15.64685969</v>
@@ -4903,7 +4909,7 @@
         <v>2892</v>
       </c>
       <c r="B98" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F98">
         <v>61.02906977</v>
@@ -4932,7 +4938,7 @@
         <v>2898</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D99">
         <v>19.07787966</v>
@@ -4970,7 +4976,7 @@
         <v>2900</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I100">
         <v>0</v>
@@ -4984,7 +4990,7 @@
         <v>2903</v>
       </c>
       <c r="B101" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I101">
         <v>0</v>
@@ -4995,7 +5001,7 @@
         <v>2904</v>
       </c>
       <c r="B102" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I102">
         <v>0</v>
@@ -5009,7 +5015,7 @@
         <v>2906</v>
       </c>
       <c r="B103" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="I103">
         <v>0</v>
@@ -5023,7 +5029,7 @@
         <v>2924</v>
       </c>
       <c r="B104" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D104">
         <v>4.273957238</v>
@@ -5061,7 +5067,7 @@
         <v>2939</v>
       </c>
       <c r="B105" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D105">
         <v>1.744518349</v>
@@ -5099,7 +5105,7 @@
         <v>2960</v>
       </c>
       <c r="B106" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D106">
         <v>3.048531032</v>
@@ -5137,7 +5143,7 @@
         <v>2962</v>
       </c>
       <c r="B107" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="I107">
         <v>0</v>
@@ -5151,7 +5157,7 @@
         <v>2963</v>
       </c>
       <c r="B108" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I108">
         <v>0</v>
@@ -5165,7 +5171,7 @@
         <v>2966</v>
       </c>
       <c r="B109" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I109">
         <v>0</v>
@@ -5179,7 +5185,7 @@
         <v>2975</v>
       </c>
       <c r="B110" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D110">
         <v>7.696728709</v>
@@ -5217,7 +5223,7 @@
         <v>2977</v>
       </c>
       <c r="B111" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D111">
         <v>5.45046135</v>
@@ -5255,7 +5261,7 @@
         <v>3001</v>
       </c>
       <c r="B112" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D112">
         <v>9.158551860999999</v>
@@ -5293,7 +5299,7 @@
         <v>3003</v>
       </c>
       <c r="B113" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D113">
         <v>12.18496186</v>
@@ -5331,7 +5337,7 @@
         <v>3006</v>
       </c>
       <c r="B114" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D114">
         <v>7.77230537</v>
@@ -5369,7 +5375,7 @@
         <v>3015</v>
       </c>
       <c r="B115" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I115">
         <v>0</v>
@@ -5383,7 +5389,7 @@
         <v>3020</v>
       </c>
       <c r="B116" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D116">
         <v>21.28924473</v>
@@ -5421,7 +5427,7 @@
         <v>3032</v>
       </c>
       <c r="B117" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D117">
         <v>5.189886074</v>
@@ -5459,7 +5465,7 @@
         <v>3035</v>
       </c>
       <c r="B118" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D118">
         <v>-4.781815035</v>
@@ -5497,7 +5503,7 @@
         <v>3048</v>
       </c>
       <c r="B119" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D119">
         <v>0.192875459</v>
@@ -5535,7 +5541,7 @@
         <v>3076</v>
       </c>
       <c r="B120" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D120">
         <v>21.32764629</v>
@@ -5573,7 +5579,7 @@
         <v>3088</v>
       </c>
       <c r="B121" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I121">
         <v>0</v>
@@ -5587,7 +5593,7 @@
         <v>3128</v>
       </c>
       <c r="B122" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D122">
         <v>9.962184555</v>
@@ -5625,7 +5631,7 @@
         <v>3131</v>
       </c>
       <c r="B123" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F123">
         <v>67.07736626000001</v>
@@ -5654,7 +5660,7 @@
         <v>3150</v>
       </c>
       <c r="B124" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D124">
         <v>12.92572148</v>
@@ -5692,10 +5698,10 @@
         <v>3151</v>
       </c>
       <c r="B125" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C125" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F125">
         <v>64.99233034</v>
@@ -5724,7 +5730,7 @@
         <v>3164</v>
       </c>
       <c r="B126" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D126">
         <v>27.0709471</v>
@@ -5762,7 +5768,7 @@
         <v>3188</v>
       </c>
       <c r="B127" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D127">
         <v>18.52022646</v>
@@ -5800,7 +5806,7 @@
         <v>3195</v>
       </c>
       <c r="B128" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I128">
         <v>0</v>
@@ -5814,7 +5820,7 @@
         <v>3197</v>
       </c>
       <c r="B129" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D129">
         <v>-32.53485343</v>
@@ -5852,7 +5858,7 @@
         <v>3201</v>
       </c>
       <c r="B130" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D130">
         <v>11.69039645</v>
@@ -5884,7 +5890,7 @@
         <v>3205</v>
       </c>
       <c r="B131" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I131">
         <v>0</v>
@@ -5898,7 +5904,7 @@
         <v>3225</v>
       </c>
       <c r="B132" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D132">
         <v>21.32659154</v>
@@ -5936,10 +5942,10 @@
         <v>3245</v>
       </c>
       <c r="B133" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C133" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D133">
         <v>2.439825691</v>
@@ -5977,7 +5983,7 @@
         <v>3252</v>
       </c>
       <c r="B134" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I134">
         <v>0</v>
@@ -5988,7 +5994,7 @@
         <v>3295</v>
       </c>
       <c r="B135" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E135">
         <v>39.32707434</v>
@@ -6023,7 +6029,7 @@
         <v>3318</v>
       </c>
       <c r="B136" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D136">
         <v>17.69909024</v>
@@ -6061,7 +6067,7 @@
         <v>3353</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I137">
         <v>0</v>
@@ -6072,7 +6078,7 @@
         <v>3362</v>
       </c>
       <c r="B138" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="I138">
         <v>0</v>
@@ -6083,7 +6089,7 @@
         <v>3366</v>
       </c>
       <c r="B139" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F139">
         <v>69.42140263</v>
@@ -6112,7 +6118,7 @@
         <v>3378</v>
       </c>
       <c r="B140" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D140">
         <v>11.7768816</v>
@@ -6150,7 +6156,7 @@
         <v>3392</v>
       </c>
       <c r="B141" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E141">
         <v>-73.88953792</v>
@@ -6185,7 +6191,7 @@
         <v>3416</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I142">
         <v>0</v>
@@ -6196,7 +6202,7 @@
         <v>3441</v>
       </c>
       <c r="B143" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D143">
         <v>-1.159343056</v>
@@ -6234,7 +6240,7 @@
         <v>3446</v>
       </c>
       <c r="B144" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D144">
         <v>15.299391</v>
@@ -6272,7 +6278,7 @@
         <v>3459</v>
       </c>
       <c r="B145" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F145">
         <v>71.02100317</v>
@@ -6301,7 +6307,7 @@
         <v>3475</v>
       </c>
       <c r="B146" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D146">
         <v>0.560289007</v>
@@ -6339,7 +6345,7 @@
         <v>3478</v>
       </c>
       <c r="B147" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I147">
         <v>0</v>
@@ -6353,7 +6359,7 @@
         <v>3494</v>
       </c>
       <c r="B148" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D148">
         <v>15.02098729</v>
@@ -6391,7 +6397,7 @@
         <v>3516</v>
       </c>
       <c r="B149" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F149">
         <v>69.72543353</v>
@@ -6423,7 +6429,7 @@
         <v>3544</v>
       </c>
       <c r="B150" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D150">
         <v>8.332236877</v>
@@ -6461,7 +6467,7 @@
         <v>3562</v>
       </c>
       <c r="B151" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D151">
         <v>24.35465816</v>
@@ -6499,7 +6505,7 @@
         <v>3604</v>
       </c>
       <c r="B152" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D152">
         <v>6.103899311</v>
@@ -6537,7 +6543,7 @@
         <v>3607</v>
       </c>
       <c r="B153" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D153">
         <v>11.4161458</v>
@@ -6575,10 +6581,10 @@
         <v>3629</v>
       </c>
       <c r="B154" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C154" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D154">
         <v>-1.264009153</v>
@@ -6616,10 +6622,10 @@
         <v>3642</v>
       </c>
       <c r="B155" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C155" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D155">
         <v>-5.3011681</v>
@@ -6657,7 +6663,7 @@
         <v>3654</v>
       </c>
       <c r="B156" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E156">
         <v>-82.2339733</v>
@@ -6692,7 +6698,7 @@
         <v>3714</v>
       </c>
       <c r="B157" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D157">
         <v>-37.99887925</v>
@@ -6730,7 +6736,7 @@
         <v>3733</v>
       </c>
       <c r="B158" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D158">
         <v>10.62366053</v>
@@ -6768,7 +6774,7 @@
         <v>3774</v>
       </c>
       <c r="B159" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D159">
         <v>4.34650618</v>
@@ -6806,7 +6812,7 @@
         <v>3776</v>
       </c>
       <c r="B160" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F160">
         <v>64.80374318</v>
@@ -6835,10 +6841,10 @@
         <v>3797</v>
       </c>
       <c r="B161" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C161" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F161">
         <v>71.10711071</v>
@@ -6867,7 +6873,7 @@
         <v>3807</v>
       </c>
       <c r="B162" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D162">
         <v>11.40112833</v>
@@ -6905,7 +6911,7 @@
         <v>3826</v>
       </c>
       <c r="B163" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D163">
         <v>-2.733000475</v>
@@ -6943,7 +6949,7 @@
         <v>3838</v>
       </c>
       <c r="B164" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E164">
         <v>-31.17368105</v>
@@ -6978,7 +6984,7 @@
         <v>3879</v>
       </c>
       <c r="B165" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F165">
         <v>67.21785182000001</v>
@@ -7010,7 +7016,7 @@
         <v>3894</v>
       </c>
       <c r="B166" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D166">
         <v>-11.50450208</v>
@@ -7048,7 +7054,7 @@
         <v>3903</v>
       </c>
       <c r="B167" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D167">
         <v>22.03607095</v>
@@ -7086,7 +7092,7 @@
         <v>3918</v>
       </c>
       <c r="B168" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D168">
         <v>-0.603762249</v>
@@ -7121,7 +7127,7 @@
         <v>3948</v>
       </c>
       <c r="B169" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D169">
         <v>17.49824831</v>
@@ -7159,7 +7165,7 @@
         <v>3998</v>
       </c>
       <c r="B170" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D170">
         <v>49.8538594</v>
@@ -7194,7 +7200,7 @@
         <v>4021</v>
       </c>
       <c r="B171" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D171">
         <v>18.52308253</v>
@@ -7232,7 +7238,7 @@
         <v>4040</v>
       </c>
       <c r="B172" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D172">
         <v>-41.07283433</v>
@@ -7270,7 +7276,7 @@
         <v>4093</v>
       </c>
       <c r="B173" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D173">
         <v>2.871407185</v>
@@ -7308,7 +7314,7 @@
         <v>4108</v>
       </c>
       <c r="B174" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D174">
         <v>3.642160288</v>
@@ -7343,7 +7349,7 @@
         <v>4113</v>
       </c>
       <c r="B175" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D175">
         <v>15.08274344</v>
@@ -7381,7 +7387,7 @@
         <v>4199</v>
       </c>
       <c r="B176" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I176">
         <v>0</v>
@@ -7395,7 +7401,7 @@
         <v>4203</v>
       </c>
       <c r="B177" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I177">
         <v>0</v>
@@ -7409,7 +7415,7 @@
         <v>4242</v>
       </c>
       <c r="B178" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D178">
         <v>3.295759817</v>
@@ -7447,7 +7453,7 @@
         <v>4248</v>
       </c>
       <c r="B179" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I179">
         <v>0</v>
@@ -7461,7 +7467,7 @@
         <v>4286</v>
       </c>
       <c r="B180" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D180">
         <v>1.15109042</v>
@@ -7499,7 +7505,7 @@
         <v>4300</v>
       </c>
       <c r="B181" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E181">
         <v>-27.07478179</v>
@@ -7534,7 +7540,7 @@
         <v>4344</v>
       </c>
       <c r="B182" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I182">
         <v>0</v>
@@ -7548,10 +7554,10 @@
         <v>4375</v>
       </c>
       <c r="B183" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C183" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E183">
         <v>-60.98814205</v>
@@ -7586,7 +7592,7 @@
         <v>4378</v>
       </c>
       <c r="B184" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D184">
         <v>-10.41197741</v>
@@ -7624,7 +7630,7 @@
         <v>4436</v>
       </c>
       <c r="B185" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E185">
         <v>5.767564958</v>
@@ -7641,7 +7647,7 @@
         <v>4441</v>
       </c>
       <c r="B186" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I186">
         <v>0</v>
@@ -7655,7 +7661,7 @@
         <v>4442</v>
       </c>
       <c r="B187" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I187">
         <v>0</v>
@@ -7669,7 +7675,7 @@
         <v>4443</v>
       </c>
       <c r="B188" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I188">
         <v>0</v>
@@ -7683,7 +7689,7 @@
         <v>4449</v>
       </c>
       <c r="B189" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I189">
         <v>0</v>
@@ -7697,7 +7703,7 @@
         <v>4454</v>
       </c>
       <c r="B190" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I190">
         <v>0</v>
@@ -7711,7 +7717,7 @@
         <v>4455</v>
       </c>
       <c r="B191" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I191">
         <v>0</v>
@@ -7725,7 +7731,7 @@
         <v>4456</v>
       </c>
       <c r="B192" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I192">
         <v>0</v>
@@ -7739,7 +7745,7 @@
         <v>4457</v>
       </c>
       <c r="B193" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I193">
         <v>0</v>
@@ -7753,7 +7759,7 @@
         <v>4461</v>
       </c>
       <c r="B194" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F194">
         <v>71.56275304</v>
@@ -7779,7 +7785,7 @@
         <v>4462</v>
       </c>
       <c r="B195" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D195">
         <v>-4.274850361</v>
@@ -7811,7 +7817,7 @@
         <v>4463</v>
       </c>
       <c r="B196" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D196">
         <v>5.121769672</v>
@@ -7843,7 +7849,7 @@
         <v>4464</v>
       </c>
       <c r="B197" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F197">
         <v>68.97703207000001</v>
@@ -7869,7 +7875,7 @@
         <v>4470</v>
       </c>
       <c r="B198" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F198">
         <v>26.74209886</v>
@@ -7895,7 +7901,7 @@
         <v>4471</v>
       </c>
       <c r="B199" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D199">
         <v>1.038785184</v>
@@ -7927,10 +7933,10 @@
         <v>4477</v>
       </c>
       <c r="B200" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C200" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D200">
         <v>8.475371336</v>
@@ -7962,7 +7968,7 @@
         <v>4482</v>
       </c>
       <c r="B201" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D201">
         <v>0.185003728</v>
@@ -7994,7 +8000,7 @@
         <v>4486</v>
       </c>
       <c r="B202" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F202">
         <v>23.16621344</v>
@@ -8020,7 +8026,7 @@
         <v>4493</v>
       </c>
       <c r="B203" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D203">
         <v>-0.044362304</v>
@@ -8049,7 +8055,7 @@
         <v>4496</v>
       </c>
       <c r="B204" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D204">
         <v>0.094924235</v>
@@ -8081,10 +8087,10 @@
         <v>4497</v>
       </c>
       <c r="B205" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C205" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D205">
         <v>0.146986101</v>
@@ -8116,7 +8122,7 @@
         <v>4498</v>
       </c>
       <c r="B206" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D206">
         <v>0.110784842</v>
@@ -8148,7 +8154,7 @@
         <v>4547</v>
       </c>
       <c r="B207" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D207">
         <v>11.8793042</v>
@@ -8180,10 +8186,10 @@
         <v>4571</v>
       </c>
       <c r="B208" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C208" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E208">
         <v>105.8924136</v>
@@ -8212,10 +8218,10 @@
         <v>4580</v>
       </c>
       <c r="B209" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C209" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D209">
         <v>1.107492632</v>
@@ -8247,10 +8253,10 @@
         <v>4603</v>
       </c>
       <c r="B210" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C210" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E210">
         <v>-43.56450971</v>
@@ -8279,7 +8285,7 @@
         <v>4611</v>
       </c>
       <c r="B211" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="M211">
         <v>1362.74</v>
@@ -8290,7 +8296,7 @@
         <v>4621</v>
       </c>
       <c r="B212" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="213" spans="1:13">
@@ -8298,7 +8304,7 @@
         <v>4623</v>
       </c>
       <c r="B213" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F213">
         <v>65.88859238000001</v>
@@ -8334,40 +8340,40 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8375,10 +8381,10 @@
         <v>2532</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D2">
         <v>12.76128466</v>
@@ -8416,10 +8422,10 @@
         <v>2700</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D3">
         <v>1.079062619</v>
@@ -8457,10 +8463,10 @@
         <v>3151</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F4">
         <v>64.99233034</v>
@@ -8489,10 +8495,10 @@
         <v>3245</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D5">
         <v>2.439825691</v>
@@ -8530,10 +8536,10 @@
         <v>3629</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D6">
         <v>-1.264009153</v>
@@ -8571,10 +8577,10 @@
         <v>3642</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D7">
         <v>-5.3011681</v>
@@ -8612,10 +8618,10 @@
         <v>3797</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C8" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F8">
         <v>71.10711071</v>
@@ -8644,10 +8650,10 @@
         <v>4375</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E9">
         <v>-60.98814205</v>
@@ -8682,10 +8688,10 @@
         <v>4477</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C10" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D10">
         <v>8.475371336</v>
@@ -8717,10 +8723,10 @@
         <v>4497</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C11" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D11">
         <v>0.146986101</v>

</xml_diff>